<commit_message>
update input data excel file
</commit_message>
<xml_diff>
--- a/input_data_spec.xlsx
+++ b/input_data_spec.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD98040-80B6-463A-9369-EED3339DACF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732EC23B-460A-43C4-9F94-54C63BA0CBF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">h_evlp!$A$1:$T$123</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'h_htc(190409用)'!$A$1:$M$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'h_htc(190409用)'!$A$1:$N$80</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">h_evlp!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'h_htc(190409用)'!$1:$1</definedName>
   </definedNames>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2407" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2540" uniqueCount="669">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -5218,10 +5218,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>boundary</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>○（複数）</t>
     <rPh sb="2" eb="4">
       <t>フクスウ</t>
@@ -5250,19 +5246,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>[境界の種類]=[外壁側]</t>
-    <rPh sb="1" eb="3">
-      <t>キョウカイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュルイ</t>
-    </rPh>
-    <rPh sb="9" eb="12">
-      <t>ガイヘキガワ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>温度差係数</t>
     <rPh sb="0" eb="3">
       <t>オンドサ</t>
@@ -5277,51 +5260,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>方位角</t>
-    <rPh sb="0" eb="3">
-      <t>ホウイカク</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>傾斜角</t>
-    <rPh sb="0" eb="3">
-      <t>ケイシャカク</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>direction_angle</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>inclination _angle</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>例（南:0, 西:90, 北:180, 東:-90）</t>
-    <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>例（水平:0, 鉛直:90）</t>
-    <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>is_radiative_heating</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>convection_rate</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>cross_vent_room</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -5331,21 +5274,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>1:内壁側
-2:外壁側
-3:地盤</t>
-    <rPh sb="2" eb="5">
-      <t>ナイヘキガワ</t>
-    </rPh>
-    <rPh sb="8" eb="11">
-      <t>ガイヘキガワ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ジバン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>室タイプ</t>
     <rPh sb="0" eb="1">
       <t>シツ</t>
@@ -5361,39 +5289,6 @@
   </si>
   <si>
     <t>next_room_type</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>[境界の種類]=[内壁側]</t>
-    <rPh sb="1" eb="3">
-      <t>キョウカイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュルイ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ウチカベ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ガワ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>日射吸収の有無</t>
-    <rPh sb="0" eb="2">
-      <t>ニッシャ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キュウシュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ウム</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>is_solar_absorbed</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -5408,85 +5303,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>thermal_thickness_type</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>熱的厚さのタイプ</t>
-    <rPh sb="0" eb="1">
-      <t>ネツ</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>テキ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>アツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>1:thin
-2:thick</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>1:薄い
-2:厚い</t>
-    <rPh sb="2" eb="3">
-      <t>ウス</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>アツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>固定公比が切り替わる
-薄い=壁, 厚い=地盤</t>
-    <rPh sb="0" eb="2">
-      <t>コテイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>コウヒ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ウス</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>カベ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>アツ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ジバン</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>不透明部位の仕様</t>
-    <rPh sb="0" eb="3">
-      <t>フトウメイ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ブイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シヨウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>opaque_spec</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>outside_emissivity</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -5579,63 +5395,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>放射吸収比率</t>
-    <rPh sb="0" eb="2">
-      <t>ホウシャ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キュウシュウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ヒリツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>radiation_absoption_ratio</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>放射暖房による放射の吸収比率</t>
-    <rPh sb="0" eb="2">
-      <t>ホウシャ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ダンボウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ホウシャ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>キュウシュウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ヒリツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>透明部位の仕様</t>
-    <rPh sb="0" eb="2">
-      <t>トウメイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ブイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>シヨウ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>opaque_part_spec</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>transparent_part_spec</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>日射熱取得率</t>
     <rPh sb="0" eb="3">
       <t>ニッシャネツ</t>
@@ -5650,29 +5409,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>日射熱透過率</t>
-    <rPh sb="0" eb="3">
-      <t>ニッシャネツ</t>
-    </rPh>
-    <rPh sb="3" eb="6">
-      <t>トウカリツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>吸収日射熱取得率</t>
-    <rPh sb="0" eb="2">
-      <t>キュウシュウ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>ニッシャネツ</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>シュトクリツ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>熱貫流率</t>
     <rPh sb="0" eb="1">
       <t>ネツ</t>
@@ -5680,14 +5416,6 @@
     <rPh sb="1" eb="4">
       <t>カンリュウリツ</t>
     </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>solar_transmittance</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>solar_absorption_ratio</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -5866,6 +5594,870 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>セツビ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>パラメータの種類
+無印：共通
+住：住宅のみ
+建：非住宅建築物のみ</t>
+    <rPh sb="6" eb="8">
+      <t>シュルイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ムイン</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ジュウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ジュウタク</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>タツル</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ジュウタク</t>
+    </rPh>
+    <rPh sb="27" eb="30">
+      <t>ケンチクブツ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>住</t>
+    <rPh sb="0" eb="1">
+      <t>ジュウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>自然風利用時の換気回数</t>
+    <rPh sb="0" eb="2">
+      <t>シゼン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>フウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>カンキカイスウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>natural_vent_time</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1:間仕切り
+2:外皮
+3:地盤</t>
+    <rPh sb="2" eb="5">
+      <t>マジキ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガイヒ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ジバン</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[境界の種類]=[外皮]</t>
+    <rPh sb="1" eb="3">
+      <t>キョウカイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シュルイ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ガイヒ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[境界の種類]=[間仕切り]</t>
+    <rPh sb="1" eb="3">
+      <t>キョウカイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シュルイ</t>
+    </rPh>
+    <rPh sb="9" eb="12">
+      <t>マジキ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>非住宅の場合は、常に間仕切りの向こう側は等温制御にするため指定不要</t>
+    <rPh sb="0" eb="3">
+      <t>ヒジュウタク</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ツネ</t>
+    </rPh>
+    <rPh sb="10" eb="13">
+      <t>マジキ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>トウオン</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セイギョ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>室内侵入日射吸収の有無</t>
+    <rPh sb="0" eb="2">
+      <t>シツナイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シンニュウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ニッシャ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キュウシュウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ウム</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>必ず室1つにつき1箇所は指定すること。</t>
+    <rPh sb="0" eb="1">
+      <t>カナラ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>シツ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>カショ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>一般部位の仕様</t>
+    <rPh sb="0" eb="2">
+      <t>イッパン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ブイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>general_part_spec</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>boundaries</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>透明な開口部の仕様</t>
+    <rPh sb="0" eb="2">
+      <t>トウメイ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>カイコウブ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>不透明な開口部の仕様</t>
+    <rPh sb="0" eb="3">
+      <t>フトウメイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>カイコウブ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>transient_opening_part</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>opaque_opening_part</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>入力方法</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>input_method</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1:simple
+2:detailed</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>simple:従来住宅で使用してきたもの
+detailed:従来非住宅で使用してきたもの</t>
+    <rPh sb="7" eb="9">
+      <t>ジュウライ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ジュウタク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ジュウライ</t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t>ヒジュウタク</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1:簡易法
+2:詳細法</t>
+    <rPh sb="2" eb="4">
+      <t>カンイ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[入力方法]=[簡易法]</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>カンイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>[入力方法]=[詳細法]</t>
+    <rPh sb="1" eb="3">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ホウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>x1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>x2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>x3</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>y1</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>y2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>y3</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>z_y_pls</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>z_x_pls</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>z_x_mns</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>z_y_mns</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>窓幅</t>
+    <rPh sb="0" eb="1">
+      <t>マド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ハバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>窓高さ</t>
+    <rPh sb="0" eb="1">
+      <t>マド</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>側壁右の出幅</t>
+    <rPh sb="0" eb="2">
+      <t>ソクヘキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ミギ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>デハバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>側壁左の出幅</t>
+    <rPh sb="0" eb="2">
+      <t>ソクヘキ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒダリ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>デハバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>庇水平方向の出(左)</t>
+    <rPh sb="0" eb="1">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="1" eb="5">
+      <t>スイヘイホウコウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ヒダリ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>庇水平方向の出(右)</t>
+    <rPh sb="0" eb="1">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="1" eb="5">
+      <t>スイヘイホウコウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>上部庇の窓上端からの距離</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウブ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>マド</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ジョウタン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>下部庇の窓下端からの距離</t>
+    <rPh sb="0" eb="2">
+      <t>カブ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>マド</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カタン</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>上部庇の出幅</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウブ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>デハバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>下部庇の出幅</t>
+    <rPh sb="0" eb="2">
+      <t>カブ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ヒサシ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>デハバ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>暖房時設定温度</t>
+    <rPh sb="0" eb="3">
+      <t>ダンボウジ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>セッテイオンド</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>△</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>要素数8760のリスト型</t>
+    <rPh sb="0" eb="2">
+      <t>ヨウソ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ガタ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>℃</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>冷房時設定温度</t>
+    <rPh sb="0" eb="3">
+      <t>レイボウジ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>セッテイオンド</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>冷房時設定相対湿度</t>
+    <rPh sb="0" eb="3">
+      <t>レイボウジ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="5" eb="9">
+      <t>ソウタイシツド</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>heating_set_temperatures</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>cooling_set_temperatures</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>cooling_set_relative_humidity</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>スケジュール</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>schedule</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>照明内部発熱</t>
+    <rPh sb="0" eb="2">
+      <t>ショウメイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ハツネツ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>heat_generation_lighting</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>局所換気量</t>
+    <rPh sb="0" eb="2">
+      <t>キョクショ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>カンキリョウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>local_vent_amount</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>m3/h</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>在室人数</t>
+    <rPh sb="0" eb="2">
+      <t>ザイシツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ニンズウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>number_of_people</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>－</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>機器内部発熱</t>
+    <rPh sb="0" eb="2">
+      <t>キキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ハツネツ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>heat_generation_appliances</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>調理内部発熱</t>
+    <rPh sb="0" eb="2">
+      <t>チョウリ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ハツネツ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>調理内部発湿</t>
+    <rPh sb="0" eb="2">
+      <t>チョウリ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ハッ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>シツ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>heat_generation_cooking</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>humidigy_generation_cooking</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>kg/kgDA</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>以下、設備関係、未作業（非住宅は不要）</t>
+    <rPh sb="0" eb="2">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セツビ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カンケイ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>ミサギョウ</t>
+    </rPh>
+    <rPh sb="12" eb="15">
+      <t>ヒジュウタク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>フヨウ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>List[float]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>List[int]</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>向き</t>
+    <rPh sb="0" eb="1">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>8方位＋上・下
+s, sw, w, nw, n, ne, e, se, top, bottom</t>
+    <rPh sb="1" eb="3">
+      <t>ホウイ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>シタ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>日射の有無</t>
+    <rPh sb="0" eb="2">
+      <t>ニッシャ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ウム</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1: 当たる
+2: 当たらない</t>
+    <rPh sb="3" eb="4">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>is_solar_absorbed_inside</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>is_sun_striked_outside</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1:s
+2:sw
+3:w
+4:nw
+5:n
+6:ne
+7:e
+8:se
+9:top
+10:bottom</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1:南
+2:南西
+3:西
+4:北西
+5:北
+6:北東
+7:東
+8:南東
+9:上
+10:下</t>
+    <rPh sb="2" eb="3">
+      <t>ミナミ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ナンセイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ニシ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ホクセイ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>キタ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ホクトウ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ヒガシ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ナントウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>シタ</t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>str</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [日射の有無]=[当たる]</t>
+    <rPh sb="2" eb="4">
+      <t>ニッッシャ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ウム</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ア</t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -16434,36 +17026,37 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A158" sqref="A158"/>
       <selection pane="topRight" activeCell="A158" sqref="A158"/>
       <selection pane="bottomLeft" activeCell="A158" sqref="A158"/>
-      <selection pane="bottomRight" activeCell="P75" sqref="P75"/>
+      <selection pane="bottomRight" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999"/>
   <cols>
     <col min="1" max="2" width="3.25" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.9375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.8125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.3125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.8125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.9375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="17" style="2" customWidth="1"/>
-    <col min="19" max="19" width="23.1875" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="2"/>
+    <col min="13" max="13" width="20.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.9375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="17" style="2" customWidth="1"/>
+    <col min="20" max="20" width="23.1875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="52.9">
+    <row r="1" spans="1:14" ht="70.5">
       <c r="A1" s="30" t="s">
         <v>13</v>
       </c>
@@ -16493,10 +17086,13 @@
         <v>5</v>
       </c>
       <c r="M1" s="5" t="s">
+        <v>580</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -16518,8 +17114,9 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" ht="141">
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:14" ht="141">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>14</v>
@@ -16543,16 +17140,17 @@
         <v>10</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>653</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>14</v>
@@ -16572,14 +17170,15 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>464</v>
       </c>
       <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -16601,8 +17200,9 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>14</v>
@@ -16622,16 +17222,17 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>53</v>
+        <v>655</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="70.5">
+    <row r="7" spans="1:14" ht="70.5">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -16640,7 +17241,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>427</v>
@@ -16655,16 +17256,19 @@
         <v>171</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>167</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
@@ -16684,14 +17288,15 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>460</v>
       </c>
       <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>14</v>
@@ -16711,14 +17316,15 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>473</v>
       </c>
       <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
@@ -16739,9 +17345,12 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="M10" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -16761,14 +17370,17 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>53</v>
+        <v>655</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="M11" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
@@ -16788,14 +17400,17 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="M12" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
@@ -16815,14 +17430,17 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="M13" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>14</v>
@@ -16831,332 +17449,344 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>481</v>
+        <v>582</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>546</v>
+        <v>583</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>447</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1" t="s">
-        <v>472</v>
-      </c>
+      <c r="K14" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L14" s="1"/>
       <c r="M14" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>581</v>
+      </c>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>487</v>
+        <v>624</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>545</v>
+        <v>630</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>447</v>
+        <v>625</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>656</v>
+      </c>
       <c r="L16" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13">
+        <v>627</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1" t="s">
-        <v>534</v>
+        <v>629</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>52</v>
+        <v>632</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>447</v>
+        <v>625</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1" t="s">
-        <v>53</v>
+        <v>656</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>472</v>
+        <v>633</v>
       </c>
       <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" ht="52.9">
+      <c r="N18" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>532</v>
+        <v>637</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>533</v>
+        <v>638</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>548</v>
-      </c>
+        <v>625</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>11</v>
+        <v>656</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>472</v>
+        <v>634</v>
       </c>
       <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1" t="s">
-        <v>68</v>
+        <v>645</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>69</v>
+        <v>646</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>447</v>
+        <v>625</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>656</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>569</v>
+        <v>634</v>
       </c>
       <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>536</v>
+        <v>647</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>537</v>
+        <v>649</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>535</v>
+        <v>625</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>656</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>472</v>
+        <v>634</v>
       </c>
       <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>538</v>
+        <v>648</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>540</v>
+        <v>650</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>535</v>
+        <v>625</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>19</v>
+        <v>656</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+        <v>651</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>539</v>
+        <v>642</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>541</v>
+        <v>643</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>535</v>
+        <v>625</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1" t="s">
-        <v>19</v>
+        <v>657</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
+        <v>644</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>539</v>
+        <v>639</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>541</v>
+        <v>640</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>535</v>
+        <v>625</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1" t="s">
-        <v>19</v>
+        <v>656</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="70.5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" ht="35.25">
+        <v>641</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>14</v>
@@ -17165,29 +17795,26 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>554</v>
+        <v>52</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>555</v>
-      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>167</v>
+        <v>472</v>
       </c>
       <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" ht="35.25">
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="1:14" ht="52.9">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>14</v>
@@ -17196,31 +17823,30 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>556</v>
+        <v>532</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>447</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>559</v>
+        <v>584</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
+        <v>472</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>14</v>
@@ -17229,10 +17855,10 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>574</v>
+        <v>68</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>575</v>
+        <v>69</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>447</v>
@@ -17240,178 +17866,211 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M28" s="1" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+        <v>549</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" spans="1:14" ht="35.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>565</v>
+        <v>534</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>563</v>
+        <v>535</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>447</v>
+        <v>585</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>167</v>
+        <v>472</v>
       </c>
       <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:14" ht="176.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>566</v>
+        <v>658</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>564</v>
+        <v>66</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
+        <v>668</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>665</v>
+      </c>
       <c r="K31" s="1" t="s">
-        <v>19</v>
+        <v>655</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>167</v>
+        <v>472</v>
       </c>
       <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="N31" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="70.5">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="B32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>568</v>
+        <v>540</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>567</v>
+        <v>541</v>
       </c>
       <c r="H32" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="35.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="I33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>186</v>
+        <v>545</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>193</v>
+        <v>543</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>447</v>
@@ -17419,26 +18078,27 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="1:13">
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>571</v>
+        <v>546</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>572</v>
+        <v>544</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>447</v>
@@ -17446,74 +18106,79 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>573</v>
+        <v>167</v>
       </c>
       <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1"/>
-      <c r="B37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>582</v>
+        <v>51</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>585</v>
+        <v>52</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>447</v>
@@ -17521,26 +18186,25 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>167</v>
-      </c>
+        <v>655</v>
+      </c>
+      <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="1:13">
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>583</v>
+        <v>186</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>586</v>
+        <v>193</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>447</v>
@@ -17548,26 +18212,27 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>584</v>
+        <v>551</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>72</v>
+        <v>552</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>447</v>
@@ -17575,41 +18240,37 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>48</v>
+        <v>553</v>
       </c>
       <c r="M41" s="1"/>
-    </row>
-    <row r="42" spans="1:13">
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M42" s="1"/>
-    </row>
-    <row r="43" spans="1:13">
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
@@ -17618,10 +18279,10 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>447</v>
@@ -17629,14 +18290,15 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>167</v>
       </c>
       <c r="M43" s="1"/>
-    </row>
-    <row r="44" spans="1:13">
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
@@ -17645,10 +18307,10 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>567</v>
+        <v>72</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>447</v>
@@ -17656,14 +18318,15 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1" t="s">
-        <v>19</v>
+        <v>654</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
       <c r="M44" s="1"/>
-    </row>
-    <row r="45" spans="1:13" ht="35.25">
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
@@ -17672,48 +18335,54 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
-        <v>587</v>
+        <v>545</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>588</v>
+        <v>543</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>590</v>
-      </c>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
       <c r="K45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45" s="1"/>
+        <v>654</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="M45" s="1"/>
-    </row>
-    <row r="46" spans="1:13">
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="1"/>
-      <c r="B46" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="s">
-        <v>591</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>592</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-    </row>
-    <row r="47" spans="1:13" ht="35.25">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="1:14" ht="35.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
@@ -17722,54 +18391,50 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>593</v>
+        <v>557</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>594</v>
+        <v>558</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>447</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>75</v>
+        <v>559</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>595</v>
+        <v>560</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>11</v>
+        <v>655</v>
       </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47" s="1"/>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1" t="s">
+      <c r="B48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M48" s="1"/>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
@@ -17778,10 +18443,10 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>598</v>
+        <v>545</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>600</v>
+        <v>543</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>447</v>
@@ -17789,14 +18454,15 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1" t="s">
-        <v>11</v>
+        <v>654</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="M49" s="1"/>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
@@ -17805,10 +18471,10 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
-        <v>599</v>
+        <v>546</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>601</v>
+        <v>544</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>447</v>
@@ -17816,242 +18482,850 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1" t="s">
-        <v>11</v>
+        <v>654</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="M50" s="1"/>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N50" s="1"/>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" s="1"/>
-      <c r="B52" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="H52" s="4" t="s">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="B53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
-        <v>606</v>
+        <v>561</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>447</v>
-      </c>
+        <v>562</v>
+      </c>
+      <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53" s="4"/>
+    </row>
+    <row r="54" spans="1:14" ht="35.25">
       <c r="A54" s="1"/>
-      <c r="B54" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4" t="s">
-        <v>608</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="H54" s="4" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="I54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="1:14" ht="35.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="H55" s="4" t="s">
+      <c r="C55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="4"/>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="I55" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" s="1"/>
-      <c r="B57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="G57" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="C58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14">
       <c r="A59" s="1"/>
-      <c r="B59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>608</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="1:14">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4" t="s">
+      <c r="C60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="H61" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="H60" s="4" t="s">
+      <c r="H62" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+    </row>
+    <row r="65" spans="1:14">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+    </row>
+    <row r="70" spans="1:14">
+      <c r="N70" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="1"/>
+      <c r="B72" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H72" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-      <c r="M60" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I73" s="4"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="1"/>
+      <c r="B74" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+    </row>
+    <row r="76" spans="1:14">
+      <c r="A76" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+    </row>
+    <row r="77" spans="1:14">
+      <c r="A77" s="1"/>
+      <c r="B77" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+    </row>
+    <row r="78" spans="1:14">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="1"/>
+      <c r="B79" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I79" s="4"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="I80" s="4"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+    </row>
+    <row r="81" spans="1:14">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M81" s="1"/>
+      <c r="N81" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M82" s="1"/>
+      <c r="N82" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="N83" s="1"/>
+    </row>
+    <row r="84" spans="1:14">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="N84" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18059,7 +19333,7 @@
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>